<commit_message>
minor fix: modifies sample files
</commit_message>
<xml_diff>
--- a/public/employees.xlsx
+++ b/public/employees.xlsx
@@ -34,7 +34,7 @@
     <t xml:space="preserve">kiran</t>
   </si>
   <si>
-    <t xml:space="preserve">kirand@joshsoftware.com</t>
+    <t xml:space="preserve">kirand@dummysoftware.com</t>
   </si>
 </sst>
 </file>
@@ -145,12 +145,14 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.9234693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -172,12 +174,12 @@
         <v>4</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>9421215727</v>
+        <v>9876543210</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="kirand@joshsoftware.com"/>
+    <hyperlink ref="B2" r:id="rId1" display="kirand@dummysoftware.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>